<commit_message>
add another figure and some text
</commit_message>
<xml_diff>
--- a/stupidNE/NE prison stats.xlsx
+++ b/stupidNE/NE prison stats.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15825" windowHeight="6735"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15825" windowHeight="6735" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="prison stats" sheetId="1" r:id="rId1"/>
+    <sheet name="arrest stats" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
   <si>
     <t>year</t>
   </si>
@@ -51,6 +52,9 @@
   </si>
   <si>
     <t>Poss except MJ</t>
+  </si>
+  <si>
+    <t>drug-related arrests</t>
   </si>
 </sst>
 </file>
@@ -218,7 +222,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$4:$A$11</c:f>
+              <c:f>'prison stats'!$A$4:$A$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -251,7 +255,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$I$4:$I$11</c:f>
+              <c:f>'prison stats'!$I$4:$I$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -292,11 +296,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2029883504"/>
-        <c:axId val="2056474192"/>
+        <c:axId val="2029891120"/>
+        <c:axId val="2029884592"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2029883504"/>
+        <c:axId val="2029891120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -392,12 +396,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2056474192"/>
+        <c:crossAx val="2029884592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2056474192"/>
+        <c:axId val="2029884592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="400"/>
@@ -435,7 +439,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2029883504"/>
+        <c:crossAx val="2029891120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -620,7 +624,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$4:$A$11</c:f>
+              <c:f>'prison stats'!$A$4:$A$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -653,7 +657,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$4:$E$11</c:f>
+              <c:f>'prison stats'!$E$4:$E$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -694,11 +698,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2099809856"/>
-        <c:axId val="2029893296"/>
+        <c:axId val="2029881328"/>
+        <c:axId val="2029885136"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2099809856"/>
+        <c:axId val="2029881328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -794,12 +798,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2029893296"/>
+        <c:crossAx val="2029885136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2029893296"/>
+        <c:axId val="2029885136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="20"/>
@@ -837,7 +841,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2099809856"/>
+        <c:crossAx val="2029881328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -847,6 +851,518 @@
           <a:solidFill>
             <a:schemeClr val="tx1"/>
           </a:solidFill>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>NE</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> D</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>rug-related arrests</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.104580927384077"/>
+          <c:y val="0.17171296296296296"/>
+          <c:w val="0.83953018372703414"/>
+          <c:h val="0.68290135608048985"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'arrest stats'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>drug-related arrests</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'arrest stats'!$A$2:$A$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>1994</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1995</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1996</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1997</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2003</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2005</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2014</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'arrest stats'!$B$2:$B$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>5452</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6594</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7765</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9197</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9014</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9288</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10166</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11263</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12042</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10278</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10905</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11299</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>10597</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>10323</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>10541</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>10132</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>10201</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>10045</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>10518</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>10629</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>12022</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2059319808"/>
+        <c:axId val="2059318176"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2059319808"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Year</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2059318176"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2059318176"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2059319808"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
         </a:ln>
         <a:effectLst/>
       </c:spPr>
@@ -968,6 +1484,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -1981,6 +2537,522 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -2057,6 +3129,41 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>195262</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>500062</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>138112</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2330,7 +3437,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
@@ -2612,4 +3719,196 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1994</v>
+      </c>
+      <c r="B2">
+        <v>5452</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1995</v>
+      </c>
+      <c r="B3">
+        <v>6594</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1996</v>
+      </c>
+      <c r="B4">
+        <v>7765</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1997</v>
+      </c>
+      <c r="B5">
+        <v>9197</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1998</v>
+      </c>
+      <c r="B6">
+        <v>9014</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1999</v>
+      </c>
+      <c r="B7">
+        <v>9288</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>2000</v>
+      </c>
+      <c r="B8">
+        <v>10166</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>2001</v>
+      </c>
+      <c r="B9">
+        <v>11263</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>2002</v>
+      </c>
+      <c r="B10">
+        <v>12042</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>2003</v>
+      </c>
+      <c r="B11">
+        <v>10278</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>2004</v>
+      </c>
+      <c r="B12">
+        <v>10905</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>2005</v>
+      </c>
+      <c r="B13">
+        <v>11299</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>2006</v>
+      </c>
+      <c r="B14">
+        <v>10597</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>2007</v>
+      </c>
+      <c r="B15">
+        <v>10323</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>2008</v>
+      </c>
+      <c r="B16">
+        <v>10541</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>2009</v>
+      </c>
+      <c r="B17">
+        <v>10132</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>2010</v>
+      </c>
+      <c r="B18">
+        <v>10201</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>2011</v>
+      </c>
+      <c r="B19">
+        <v>10045</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>2012</v>
+      </c>
+      <c r="B20">
+        <v>10518</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>2013</v>
+      </c>
+      <c r="B21">
+        <v>10629</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>2014</v>
+      </c>
+      <c r="B22">
+        <v>12022</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fixed graphs and figure bordesrs
</commit_message>
<xml_diff>
--- a/stupidNE/NE prison stats.xlsx
+++ b/stupidNE/NE prison stats.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15825" windowHeight="6735" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15825" windowHeight="6735"/>
   </bookViews>
   <sheets>
     <sheet name="prison stats" sheetId="1" r:id="rId1"/>
@@ -149,6 +149,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -295,11 +296,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2099805504"/>
-        <c:axId val="2099809312"/>
+        <c:axId val="2059128992"/>
+        <c:axId val="2059130624"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2099805504"/>
+        <c:axId val="2059128992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -331,6 +332,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -394,12 +396,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2099809312"/>
+        <c:crossAx val="2059130624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2099809312"/>
+        <c:axId val="2059130624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="400"/>
@@ -437,7 +439,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2099805504"/>
+        <c:crossAx val="2059128992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -460,12 +462,7 @@
       <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
+      <a:noFill/>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -536,19 +533,12 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Possession of drugs</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> (</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>assuming marijuana)</a:t>
+              <a:t>Sale, manufacture, or distribution of drugs </a:t>
             </a:r>
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -695,11 +685,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2099808768"/>
-        <c:axId val="2099807680"/>
+        <c:axId val="2054412176"/>
+        <c:axId val="2054409456"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2099808768"/>
+        <c:axId val="2054412176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -731,6 +721,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -794,12 +785,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2099807680"/>
+        <c:crossAx val="2054409456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2099807680"/>
+        <c:axId val="2054409456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="20"/>
@@ -837,7 +828,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2099808768"/>
+        <c:crossAx val="2054412176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -860,12 +851,7 @@
       <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
+      <a:noFill/>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -1172,11 +1158,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2099808224"/>
-        <c:axId val="2062411776"/>
+        <c:axId val="2103407696"/>
+        <c:axId val="2103404432"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2099808224"/>
+        <c:axId val="2103407696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2014"/>
@@ -1291,12 +1277,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2062411776"/>
+        <c:crossAx val="2103404432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2062411776"/>
+        <c:axId val="2103404432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="4000"/>
@@ -1354,7 +1340,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2099808224"/>
+        <c:crossAx val="2103407696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1375,12 +1361,7 @@
       <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
+      <a:noFill/>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -3436,7 +3417,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:J11"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
       <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
@@ -3724,7 +3705,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>

</xml_diff>